<commit_message>
Evol 835: import, export, copy/paste fixed
</commit_message>
<xml_diff>
--- a/integration-tests/src/it/resources/import/import-requirement.xlsx
+++ b/integration-tests/src/it/resources/import/import-requirement.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>PATH</t>
   </si>
@@ -192,9 +192,6 @@
     <t>COMMENTAIRE</t>
   </si>
   <si>
-    <t>version dans le desordre</t>
-  </si>
-  <si>
     <t>name4/name//5</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
   </si>
   <si>
     <t>version-1</t>
-  </si>
-  <si>
-    <t>will be renamed</t>
   </si>
   <si>
     <t>version in order</t>
@@ -232,12 +226,39 @@
   <si>
     <t>description</t>
   </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>FUNCTIONAL</t>
+  </si>
+  <si>
+    <t>NON_FUNCTIONAL</t>
+  </si>
+  <si>
+    <t>BUSINESS</t>
+  </si>
+  <si>
+    <t>TEST_REQUIREMENT</t>
+  </si>
+  <si>
+    <t>USE_CASE</t>
+  </si>
+  <si>
+    <t>version not in order</t>
+  </si>
+  <si>
+    <t>date will be today but do not create error</t>
+  </si>
+  <si>
+    <t>will be renamed because of homonyme folder</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,8 +317,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +334,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -440,6 +479,17 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,29 +852,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K241"/>
+  <dimension ref="A1:L241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" style="16" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="15" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="16" customWidth="1"/>
-    <col min="10" max="10" width="16" style="16" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="15" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="16"/>
+    <col min="5" max="6" width="20.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" style="16" customWidth="1"/>
+    <col min="11" max="11" width="16" style="16" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="15" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="12" customFormat="1" ht="12">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:12" s="12" customFormat="1" ht="12">
+      <c r="A1" s="27" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -840,27 +890,30 @@
         <v>3</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="12">
+    <row r="2" spans="1:12" ht="12">
       <c r="A2" s="16" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>30</v>
@@ -872,22 +925,28 @@
         <v>6</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="24">
         <v>20510</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="26">
+      <c r="I2" s="11"/>
+      <c r="J2" s="26">
         <v>30861</v>
       </c>
-      <c r="J2" s="10"/>
       <c r="K2" s="10"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" ht="12">
+      <c r="A3" s="25" t="s">
+        <v>69</v>
+      </c>
       <c r="B3" s="10" t="s">
         <v>30</v>
       </c>
@@ -898,29 +957,32 @@
         <v>2</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="9"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="10">
+      <c r="L3" s="10">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="12">
+    <row r="4" spans="1:12" ht="12">
       <c r="A4" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -928,24 +990,27 @@
         <v>57</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="26">
+      <c r="J4" s="26">
         <v>30858</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="12">
+    <row r="5" spans="1:12" ht="12">
       <c r="A5" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>31</v>
@@ -956,37 +1021,44 @@
         <v>48</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="26">
+      <c r="I5" s="11"/>
+      <c r="J5" s="26">
         <v>30859</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="12">
-      <c r="A6" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" ht="12">
+    <row r="6" spans="1:12" s="31" customFormat="1" ht="12">
+      <c r="A6" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+    </row>
+    <row r="7" spans="1:12" ht="12">
       <c r="A7" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>35</v>
@@ -998,24 +1070,27 @@
       <c r="E7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="26">
+      <c r="I7" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="26">
         <v>30860</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10">
+      <c r="K7" s="10"/>
+      <c r="L7" s="10">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="12">
+    <row r="8" spans="1:12" ht="12">
       <c r="A8" s="16"/>
       <c r="B8" s="10" t="s">
         <v>35</v>
@@ -1027,26 +1102,27 @@
       <c r="E8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10" t="s">
+      <c r="I8" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="L8" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="12">
+    <row r="9" spans="1:12" ht="12">
       <c r="A9" s="16" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>38</v>
@@ -1060,1960 +1136,1964 @@
       <c r="E9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="10"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L9" s="10"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="17"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="17"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="17"/>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="17"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="2:11">
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="2:11">
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="2:11">
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="2:11">
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" spans="2:12">
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="17"/>
-    </row>
-    <row r="21" spans="2:11">
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" spans="2:12">
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="17"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22" spans="2:12">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="17"/>
-    </row>
-    <row r="23" spans="2:11">
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="2:12">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="2:11">
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="2:12">
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="17"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="17"/>
-    </row>
-    <row r="25" spans="2:11">
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="2:12">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="17"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="17"/>
-    </row>
-    <row r="26" spans="2:11">
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="2:12">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="17"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="17"/>
-    </row>
-    <row r="27" spans="2:11">
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="2:12">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="17"/>
-    </row>
-    <row r="28" spans="2:11">
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="2:12">
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="17"/>
-    </row>
-    <row r="29" spans="2:11">
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="2:12">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="17"/>
-      <c r="K29" s="18"/>
-    </row>
-    <row r="30" spans="2:11">
+      <c r="I29" s="17"/>
+      <c r="L29" s="18"/>
+    </row>
+    <row r="30" spans="2:12">
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="17"/>
-      <c r="K30" s="18"/>
-    </row>
-    <row r="31" spans="2:11">
+      <c r="I30" s="17"/>
+      <c r="L30" s="18"/>
+    </row>
+    <row r="31" spans="2:12">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="17"/>
-      <c r="K31" s="18"/>
-    </row>
-    <row r="32" spans="2:11">
+      <c r="I31" s="17"/>
+      <c r="L31" s="18"/>
+    </row>
+    <row r="32" spans="2:12">
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="17"/>
+      <c r="G32" s="18"/>
       <c r="H32" s="17"/>
-      <c r="K32" s="18"/>
-    </row>
-    <row r="33" spans="2:11">
+      <c r="I32" s="17"/>
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="2:12">
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="17"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="17"/>
-      <c r="K33" s="18"/>
-    </row>
-    <row r="34" spans="2:11">
+      <c r="I33" s="17"/>
+      <c r="L33" s="18"/>
+    </row>
+    <row r="34" spans="2:12">
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="17"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="17"/>
-      <c r="K34" s="18"/>
-    </row>
-    <row r="35" spans="2:11">
+      <c r="I34" s="17"/>
+      <c r="L34" s="18"/>
+    </row>
+    <row r="35" spans="2:12">
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="17"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="17"/>
-      <c r="K35" s="18"/>
-    </row>
-    <row r="36" spans="2:11">
+      <c r="I35" s="17"/>
+      <c r="L35" s="18"/>
+    </row>
+    <row r="36" spans="2:12">
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="17"/>
-      <c r="K36" s="18"/>
-    </row>
-    <row r="37" spans="2:11">
+      <c r="I36" s="17"/>
+      <c r="L36" s="18"/>
+    </row>
+    <row r="37" spans="2:12">
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="17"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="17"/>
-      <c r="K37" s="18"/>
-    </row>
-    <row r="38" spans="2:11">
+      <c r="I37" s="17"/>
+      <c r="L37" s="18"/>
+    </row>
+    <row r="38" spans="2:12">
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="17"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="17"/>
-      <c r="K38" s="18"/>
-    </row>
-    <row r="39" spans="2:11">
+      <c r="I38" s="17"/>
+      <c r="L38" s="18"/>
+    </row>
+    <row r="39" spans="2:12">
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="17"/>
-      <c r="K39" s="18"/>
-    </row>
-    <row r="40" spans="2:11">
+      <c r="I39" s="17"/>
+      <c r="L39" s="18"/>
+    </row>
+    <row r="40" spans="2:12">
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="18"/>
       <c r="H40" s="17"/>
-      <c r="K40" s="18"/>
-    </row>
-    <row r="41" spans="2:11">
+      <c r="I40" s="17"/>
+      <c r="L40" s="18"/>
+    </row>
+    <row r="41" spans="2:12">
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="17"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="17"/>
-      <c r="K41" s="18"/>
-    </row>
-    <row r="42" spans="2:11">
+      <c r="I41" s="17"/>
+      <c r="L41" s="18"/>
+    </row>
+    <row r="42" spans="2:12">
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="17"/>
+      <c r="G42" s="18"/>
       <c r="H42" s="17"/>
-      <c r="K42" s="18"/>
-    </row>
-    <row r="43" spans="2:11">
+      <c r="I42" s="17"/>
+      <c r="L42" s="18"/>
+    </row>
+    <row r="43" spans="2:12">
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="17"/>
+      <c r="G43" s="18"/>
       <c r="H43" s="17"/>
-      <c r="K43" s="18"/>
-    </row>
-    <row r="44" spans="2:11">
+      <c r="I43" s="17"/>
+      <c r="L43" s="18"/>
+    </row>
+    <row r="44" spans="2:12">
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="17"/>
+      <c r="G44" s="18"/>
       <c r="H44" s="17"/>
-      <c r="K44" s="18"/>
-    </row>
-    <row r="45" spans="2:11">
+      <c r="I44" s="17"/>
+      <c r="L44" s="18"/>
+    </row>
+    <row r="45" spans="2:12">
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="17"/>
+      <c r="G45" s="18"/>
       <c r="H45" s="17"/>
-      <c r="K45" s="18"/>
-    </row>
-    <row r="46" spans="2:11">
+      <c r="I45" s="17"/>
+      <c r="L45" s="18"/>
+    </row>
+    <row r="46" spans="2:12">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="17"/>
+      <c r="G46" s="18"/>
       <c r="H46" s="17"/>
-      <c r="K46" s="18"/>
-    </row>
-    <row r="47" spans="2:11">
+      <c r="I46" s="17"/>
+      <c r="L46" s="18"/>
+    </row>
+    <row r="47" spans="2:12">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="17"/>
+      <c r="G47" s="18"/>
       <c r="H47" s="17"/>
-      <c r="K47" s="18"/>
-    </row>
-    <row r="48" spans="2:11">
+      <c r="I47" s="17"/>
+      <c r="L47" s="18"/>
+    </row>
+    <row r="48" spans="2:12">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="17"/>
+      <c r="G48" s="18"/>
       <c r="H48" s="17"/>
-      <c r="K48" s="18"/>
-    </row>
-    <row r="49" spans="2:11">
+      <c r="I48" s="17"/>
+      <c r="L48" s="18"/>
+    </row>
+    <row r="49" spans="2:12">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="17"/>
+      <c r="G49" s="18"/>
       <c r="H49" s="17"/>
-      <c r="K49" s="18"/>
-    </row>
-    <row r="50" spans="2:11">
+      <c r="I49" s="17"/>
+      <c r="L49" s="18"/>
+    </row>
+    <row r="50" spans="2:12">
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="17"/>
+      <c r="G50" s="18"/>
       <c r="H50" s="17"/>
-      <c r="K50" s="18"/>
-    </row>
-    <row r="51" spans="2:11">
+      <c r="I50" s="17"/>
+      <c r="L50" s="18"/>
+    </row>
+    <row r="51" spans="2:12">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="17"/>
+      <c r="G51" s="18"/>
       <c r="H51" s="17"/>
-      <c r="K51" s="18"/>
-    </row>
-    <row r="52" spans="2:11">
+      <c r="I51" s="17"/>
+      <c r="L51" s="18"/>
+    </row>
+    <row r="52" spans="2:12">
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="17"/>
+      <c r="G52" s="18"/>
       <c r="H52" s="17"/>
-      <c r="K52" s="18"/>
-    </row>
-    <row r="53" spans="2:11">
+      <c r="I52" s="17"/>
+      <c r="L52" s="18"/>
+    </row>
+    <row r="53" spans="2:12">
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="17"/>
+      <c r="G53" s="18"/>
       <c r="H53" s="17"/>
-      <c r="K53" s="18"/>
-    </row>
-    <row r="54" spans="2:11">
+      <c r="I53" s="17"/>
+      <c r="L53" s="18"/>
+    </row>
+    <row r="54" spans="2:12">
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="17"/>
+      <c r="G54" s="18"/>
       <c r="H54" s="17"/>
-      <c r="K54" s="18"/>
-    </row>
-    <row r="55" spans="2:11">
+      <c r="I54" s="17"/>
+      <c r="L54" s="18"/>
+    </row>
+    <row r="55" spans="2:12">
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="17"/>
+      <c r="G55" s="18"/>
       <c r="H55" s="17"/>
-      <c r="K55" s="18"/>
-    </row>
-    <row r="56" spans="2:11">
+      <c r="I55" s="17"/>
+      <c r="L55" s="18"/>
+    </row>
+    <row r="56" spans="2:12">
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="17"/>
+      <c r="G56" s="18"/>
       <c r="H56" s="17"/>
-      <c r="K56" s="18"/>
-    </row>
-    <row r="57" spans="2:11">
+      <c r="I56" s="17"/>
+      <c r="L56" s="18"/>
+    </row>
+    <row r="57" spans="2:12">
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="17"/>
+      <c r="G57" s="18"/>
       <c r="H57" s="17"/>
-      <c r="K57" s="18"/>
-    </row>
-    <row r="58" spans="2:11">
+      <c r="I57" s="17"/>
+      <c r="L57" s="18"/>
+    </row>
+    <row r="58" spans="2:12">
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="17"/>
+      <c r="G58" s="18"/>
       <c r="H58" s="17"/>
-      <c r="K58" s="18"/>
-    </row>
-    <row r="59" spans="2:11">
+      <c r="I58" s="17"/>
+      <c r="L58" s="18"/>
+    </row>
+    <row r="59" spans="2:12">
       <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="17"/>
+      <c r="G59" s="18"/>
       <c r="H59" s="17"/>
-      <c r="K59" s="18"/>
-    </row>
-    <row r="60" spans="2:11">
+      <c r="I59" s="17"/>
+      <c r="L59" s="18"/>
+    </row>
+    <row r="60" spans="2:12">
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="17"/>
+      <c r="G60" s="18"/>
       <c r="H60" s="17"/>
-      <c r="K60" s="18"/>
-    </row>
-    <row r="61" spans="2:11">
+      <c r="I60" s="17"/>
+      <c r="L60" s="18"/>
+    </row>
+    <row r="61" spans="2:12">
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="17"/>
+      <c r="G61" s="18"/>
       <c r="H61" s="17"/>
-      <c r="K61" s="18"/>
-    </row>
-    <row r="62" spans="2:11">
+      <c r="I61" s="17"/>
+      <c r="L61" s="18"/>
+    </row>
+    <row r="62" spans="2:12">
       <c r="B62" s="12"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="17"/>
+      <c r="G62" s="18"/>
       <c r="H62" s="17"/>
-      <c r="K62" s="18"/>
-    </row>
-    <row r="63" spans="2:11">
+      <c r="I62" s="17"/>
+      <c r="L62" s="18"/>
+    </row>
+    <row r="63" spans="2:12">
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="17"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="17"/>
-      <c r="K63" s="18"/>
-    </row>
-    <row r="64" spans="2:11">
+      <c r="I63" s="17"/>
+      <c r="L63" s="18"/>
+    </row>
+    <row r="64" spans="2:12">
       <c r="B64" s="12"/>
       <c r="C64" s="12"/>
       <c r="D64" s="12"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="17"/>
+      <c r="G64" s="18"/>
       <c r="H64" s="17"/>
-      <c r="K64" s="18"/>
-    </row>
-    <row r="65" spans="2:11">
+      <c r="I64" s="17"/>
+      <c r="L64" s="18"/>
+    </row>
+    <row r="65" spans="2:12">
       <c r="B65" s="12"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="17"/>
+      <c r="G65" s="18"/>
       <c r="H65" s="17"/>
-      <c r="K65" s="19"/>
-    </row>
-    <row r="66" spans="2:11">
+      <c r="I65" s="17"/>
+      <c r="L65" s="19"/>
+    </row>
+    <row r="66" spans="2:12">
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="17"/>
+      <c r="G66" s="18"/>
       <c r="H66" s="17"/>
-      <c r="K66" s="19"/>
-    </row>
-    <row r="67" spans="2:11">
+      <c r="I66" s="17"/>
+      <c r="L66" s="19"/>
+    </row>
+    <row r="67" spans="2:12">
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="17"/>
+      <c r="G67" s="18"/>
       <c r="H67" s="17"/>
-      <c r="K67" s="19"/>
-    </row>
-    <row r="68" spans="2:11">
+      <c r="I67" s="17"/>
+      <c r="L67" s="19"/>
+    </row>
+    <row r="68" spans="2:12">
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="17"/>
+      <c r="G68" s="18"/>
       <c r="H68" s="17"/>
-      <c r="K68" s="19"/>
-    </row>
-    <row r="69" spans="2:11">
+      <c r="I68" s="17"/>
+      <c r="L68" s="19"/>
+    </row>
+    <row r="69" spans="2:12">
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="17"/>
+      <c r="G69" s="18"/>
       <c r="H69" s="17"/>
-      <c r="K69" s="19"/>
-    </row>
-    <row r="70" spans="2:11">
+      <c r="I69" s="17"/>
+      <c r="L69" s="19"/>
+    </row>
+    <row r="70" spans="2:12">
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="17"/>
+      <c r="G70" s="18"/>
       <c r="H70" s="17"/>
-      <c r="K70" s="19"/>
-    </row>
-    <row r="71" spans="2:11">
+      <c r="I70" s="17"/>
+      <c r="L70" s="19"/>
+    </row>
+    <row r="71" spans="2:12">
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="17"/>
+      <c r="G71" s="18"/>
       <c r="H71" s="17"/>
-      <c r="K71" s="19"/>
-    </row>
-    <row r="72" spans="2:11">
+      <c r="I71" s="17"/>
+      <c r="L71" s="19"/>
+    </row>
+    <row r="72" spans="2:12">
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="17"/>
+      <c r="G72" s="18"/>
       <c r="H72" s="17"/>
-      <c r="K72" s="19"/>
-    </row>
-    <row r="73" spans="2:11">
+      <c r="I72" s="17"/>
+      <c r="L72" s="19"/>
+    </row>
+    <row r="73" spans="2:12">
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="17"/>
+      <c r="G73" s="18"/>
       <c r="H73" s="17"/>
-      <c r="K73" s="19"/>
-    </row>
-    <row r="74" spans="2:11">
+      <c r="I73" s="17"/>
+      <c r="L73" s="19"/>
+    </row>
+    <row r="74" spans="2:12">
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="17"/>
+      <c r="G74" s="18"/>
       <c r="H74" s="17"/>
-      <c r="K74" s="19"/>
-    </row>
-    <row r="75" spans="2:11">
+      <c r="I74" s="17"/>
+      <c r="L74" s="19"/>
+    </row>
+    <row r="75" spans="2:12">
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="17"/>
+      <c r="G75" s="18"/>
       <c r="H75" s="17"/>
-      <c r="K75" s="19"/>
-    </row>
-    <row r="76" spans="2:11">
+      <c r="I75" s="17"/>
+      <c r="L75" s="19"/>
+    </row>
+    <row r="76" spans="2:12">
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="17"/>
+      <c r="G76" s="18"/>
       <c r="H76" s="17"/>
-      <c r="K76" s="19"/>
-    </row>
-    <row r="77" spans="2:11">
+      <c r="I76" s="17"/>
+      <c r="L76" s="19"/>
+    </row>
+    <row r="77" spans="2:12">
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="17"/>
+      <c r="G77" s="18"/>
       <c r="H77" s="17"/>
-      <c r="K77" s="19"/>
-    </row>
-    <row r="78" spans="2:11">
+      <c r="I77" s="17"/>
+      <c r="L77" s="19"/>
+    </row>
+    <row r="78" spans="2:12">
       <c r="B78" s="12"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="17"/>
+      <c r="G78" s="18"/>
       <c r="H78" s="17"/>
-      <c r="K78" s="19"/>
-    </row>
-    <row r="79" spans="2:11">
+      <c r="I78" s="17"/>
+      <c r="L78" s="19"/>
+    </row>
+    <row r="79" spans="2:12">
       <c r="B79" s="12"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="17"/>
+      <c r="G79" s="18"/>
       <c r="H79" s="17"/>
-      <c r="K79" s="19"/>
-    </row>
-    <row r="80" spans="2:11">
+      <c r="I79" s="17"/>
+      <c r="L79" s="19"/>
+    </row>
+    <row r="80" spans="2:12">
       <c r="B80" s="12"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="17"/>
+      <c r="G80" s="18"/>
       <c r="H80" s="17"/>
-      <c r="K80" s="19"/>
-    </row>
-    <row r="81" spans="2:11">
+      <c r="I80" s="17"/>
+      <c r="L80" s="19"/>
+    </row>
+    <row r="81" spans="2:12">
       <c r="B81" s="12"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="17"/>
+      <c r="G81" s="18"/>
       <c r="H81" s="17"/>
-      <c r="K81" s="19"/>
-    </row>
-    <row r="82" spans="2:11">
+      <c r="I81" s="17"/>
+      <c r="L81" s="19"/>
+    </row>
+    <row r="82" spans="2:12">
       <c r="B82" s="12"/>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
-      <c r="F82" s="18"/>
-      <c r="G82" s="17"/>
+      <c r="G82" s="18"/>
       <c r="H82" s="17"/>
-      <c r="K82" s="19"/>
-    </row>
-    <row r="83" spans="2:11">
+      <c r="I82" s="17"/>
+      <c r="L82" s="19"/>
+    </row>
+    <row r="83" spans="2:12">
       <c r="B83" s="12"/>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
-      <c r="F83" s="18"/>
-      <c r="G83" s="17"/>
+      <c r="G83" s="18"/>
       <c r="H83" s="17"/>
-      <c r="K83" s="19"/>
-    </row>
-    <row r="84" spans="2:11">
+      <c r="I83" s="17"/>
+      <c r="L83" s="19"/>
+    </row>
+    <row r="84" spans="2:12">
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
       <c r="D84" s="12"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="17"/>
+      <c r="G84" s="18"/>
       <c r="H84" s="17"/>
-      <c r="K84" s="18"/>
-    </row>
-    <row r="85" spans="2:11">
+      <c r="I84" s="17"/>
+      <c r="L84" s="18"/>
+    </row>
+    <row r="85" spans="2:12">
       <c r="B85" s="12"/>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="17"/>
+      <c r="G85" s="18"/>
       <c r="H85" s="17"/>
-      <c r="K85" s="18"/>
-    </row>
-    <row r="86" spans="2:11">
+      <c r="I85" s="17"/>
+      <c r="L85" s="18"/>
+    </row>
+    <row r="86" spans="2:12">
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="17"/>
+      <c r="G86" s="18"/>
       <c r="H86" s="17"/>
-      <c r="K86" s="18"/>
-    </row>
-    <row r="87" spans="2:11">
+      <c r="I86" s="17"/>
+      <c r="L86" s="18"/>
+    </row>
+    <row r="87" spans="2:12">
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="17"/>
+      <c r="G87" s="18"/>
       <c r="H87" s="17"/>
-      <c r="K87" s="18"/>
-    </row>
-    <row r="88" spans="2:11">
+      <c r="I87" s="17"/>
+      <c r="L87" s="18"/>
+    </row>
+    <row r="88" spans="2:12">
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="17"/>
+      <c r="G88" s="18"/>
       <c r="H88" s="17"/>
-      <c r="K88" s="18"/>
-    </row>
-    <row r="89" spans="2:11">
+      <c r="I88" s="17"/>
+      <c r="L88" s="18"/>
+    </row>
+    <row r="89" spans="2:12">
       <c r="B89" s="12"/>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="17"/>
+      <c r="G89" s="18"/>
       <c r="H89" s="17"/>
-      <c r="K89" s="18"/>
-    </row>
-    <row r="90" spans="2:11">
+      <c r="I89" s="17"/>
+      <c r="L89" s="18"/>
+    </row>
+    <row r="90" spans="2:12">
       <c r="B90" s="12"/>
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="17"/>
+      <c r="G90" s="18"/>
       <c r="H90" s="17"/>
-      <c r="K90" s="18"/>
-    </row>
-    <row r="91" spans="2:11">
+      <c r="I90" s="17"/>
+      <c r="L90" s="18"/>
+    </row>
+    <row r="91" spans="2:12">
       <c r="B91" s="12"/>
       <c r="C91" s="12"/>
       <c r="D91" s="12"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="17"/>
+      <c r="G91" s="18"/>
       <c r="H91" s="17"/>
-      <c r="K91" s="18"/>
-    </row>
-    <row r="92" spans="2:11">
+      <c r="I91" s="17"/>
+      <c r="L91" s="18"/>
+    </row>
+    <row r="92" spans="2:12">
       <c r="B92" s="12"/>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
-      <c r="F92" s="18"/>
-      <c r="G92" s="17"/>
+      <c r="G92" s="18"/>
       <c r="H92" s="17"/>
-      <c r="K92" s="18"/>
-    </row>
-    <row r="93" spans="2:11">
+      <c r="I92" s="17"/>
+      <c r="L92" s="18"/>
+    </row>
+    <row r="93" spans="2:12">
       <c r="B93" s="12"/>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="17"/>
+      <c r="G93" s="18"/>
       <c r="H93" s="17"/>
-      <c r="K93" s="18"/>
-    </row>
-    <row r="94" spans="2:11">
+      <c r="I93" s="17"/>
+      <c r="L93" s="18"/>
+    </row>
+    <row r="94" spans="2:12">
       <c r="B94" s="12"/>
       <c r="C94" s="12"/>
       <c r="D94" s="12"/>
-      <c r="F94" s="18"/>
-      <c r="G94" s="17"/>
+      <c r="G94" s="18"/>
       <c r="H94" s="17"/>
-      <c r="K94" s="18"/>
-    </row>
-    <row r="95" spans="2:11">
+      <c r="I94" s="17"/>
+      <c r="L94" s="18"/>
+    </row>
+    <row r="95" spans="2:12">
       <c r="B95" s="12"/>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="17"/>
+      <c r="G95" s="18"/>
       <c r="H95" s="17"/>
-      <c r="K95" s="18"/>
-    </row>
-    <row r="96" spans="2:11">
+      <c r="I95" s="17"/>
+      <c r="L95" s="18"/>
+    </row>
+    <row r="96" spans="2:12">
       <c r="B96" s="12"/>
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
-      <c r="F96" s="18"/>
-      <c r="G96" s="17"/>
+      <c r="G96" s="18"/>
       <c r="H96" s="17"/>
-      <c r="K96" s="18"/>
-    </row>
-    <row r="97" spans="2:11">
+      <c r="I96" s="17"/>
+      <c r="L96" s="18"/>
+    </row>
+    <row r="97" spans="2:12">
       <c r="B97" s="12"/>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="17"/>
+      <c r="G97" s="18"/>
       <c r="H97" s="17"/>
-      <c r="K97" s="18"/>
-    </row>
-    <row r="98" spans="2:11">
+      <c r="I97" s="17"/>
+      <c r="L97" s="18"/>
+    </row>
+    <row r="98" spans="2:12">
       <c r="B98" s="12"/>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="17"/>
+      <c r="G98" s="18"/>
       <c r="H98" s="17"/>
-      <c r="K98" s="18"/>
-    </row>
-    <row r="99" spans="2:11">
+      <c r="I98" s="17"/>
+      <c r="L98" s="18"/>
+    </row>
+    <row r="99" spans="2:12">
       <c r="B99" s="12"/>
       <c r="C99" s="12"/>
       <c r="D99" s="12"/>
-      <c r="F99" s="18"/>
-      <c r="G99" s="17"/>
+      <c r="G99" s="18"/>
       <c r="H99" s="17"/>
-      <c r="K99" s="18"/>
-    </row>
-    <row r="100" spans="2:11">
+      <c r="I99" s="17"/>
+      <c r="L99" s="18"/>
+    </row>
+    <row r="100" spans="2:12">
       <c r="B100" s="12"/>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
-      <c r="F100" s="18"/>
-      <c r="G100" s="17"/>
+      <c r="G100" s="18"/>
       <c r="H100" s="17"/>
-      <c r="K100" s="18"/>
-    </row>
-    <row r="101" spans="2:11">
+      <c r="I100" s="17"/>
+      <c r="L100" s="18"/>
+    </row>
+    <row r="101" spans="2:12">
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
       <c r="D101" s="12"/>
-      <c r="F101" s="18"/>
-      <c r="G101" s="17"/>
+      <c r="G101" s="18"/>
       <c r="H101" s="17"/>
-      <c r="K101" s="18"/>
-    </row>
-    <row r="102" spans="2:11">
+      <c r="I101" s="17"/>
+      <c r="L101" s="18"/>
+    </row>
+    <row r="102" spans="2:12">
       <c r="B102" s="12"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="17"/>
+      <c r="G102" s="18"/>
       <c r="H102" s="17"/>
-      <c r="K102" s="18"/>
-    </row>
-    <row r="103" spans="2:11">
+      <c r="I102" s="17"/>
+      <c r="L102" s="18"/>
+    </row>
+    <row r="103" spans="2:12">
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
       <c r="D103" s="12"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="17"/>
+      <c r="G103" s="18"/>
       <c r="H103" s="17"/>
-      <c r="K103" s="18"/>
-    </row>
-    <row r="104" spans="2:11">
+      <c r="I103" s="17"/>
+      <c r="L103" s="18"/>
+    </row>
+    <row r="104" spans="2:12">
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="20"/>
+      <c r="G104" s="18"/>
       <c r="H104" s="20"/>
-      <c r="K104" s="18"/>
-    </row>
-    <row r="105" spans="2:11">
+      <c r="I104" s="20"/>
+      <c r="L104" s="18"/>
+    </row>
+    <row r="105" spans="2:12">
       <c r="B105" s="12"/>
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="17"/>
+      <c r="G105" s="18"/>
       <c r="H105" s="17"/>
-      <c r="K105" s="18"/>
-    </row>
-    <row r="106" spans="2:11">
+      <c r="I105" s="17"/>
+      <c r="L105" s="18"/>
+    </row>
+    <row r="106" spans="2:12">
       <c r="B106" s="12"/>
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="17"/>
+      <c r="G106" s="18"/>
       <c r="H106" s="17"/>
-      <c r="K106" s="18"/>
-    </row>
-    <row r="107" spans="2:11">
+      <c r="I106" s="17"/>
+      <c r="L106" s="18"/>
+    </row>
+    <row r="107" spans="2:12">
       <c r="B107" s="12"/>
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
-      <c r="F107" s="18"/>
-      <c r="G107" s="17"/>
+      <c r="G107" s="18"/>
       <c r="H107" s="17"/>
-      <c r="K107" s="18"/>
-    </row>
-    <row r="108" spans="2:11">
+      <c r="I107" s="17"/>
+      <c r="L107" s="18"/>
+    </row>
+    <row r="108" spans="2:12">
       <c r="B108" s="12"/>
       <c r="C108" s="12"/>
       <c r="D108" s="12"/>
-      <c r="F108" s="18"/>
-      <c r="G108" s="17"/>
+      <c r="G108" s="18"/>
       <c r="H108" s="17"/>
-      <c r="K108" s="18"/>
-    </row>
-    <row r="109" spans="2:11">
+      <c r="I108" s="17"/>
+      <c r="L108" s="18"/>
+    </row>
+    <row r="109" spans="2:12">
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
       <c r="D109" s="12"/>
-      <c r="F109" s="18"/>
-      <c r="G109" s="17"/>
+      <c r="G109" s="18"/>
       <c r="H109" s="17"/>
-      <c r="K109" s="18"/>
-    </row>
-    <row r="110" spans="2:11">
+      <c r="I109" s="17"/>
+      <c r="L109" s="18"/>
+    </row>
+    <row r="110" spans="2:12">
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
       <c r="D110" s="12"/>
-      <c r="F110" s="18"/>
-      <c r="G110" s="17"/>
+      <c r="G110" s="18"/>
       <c r="H110" s="17"/>
-      <c r="K110" s="18"/>
-    </row>
-    <row r="111" spans="2:11">
+      <c r="I110" s="17"/>
+      <c r="L110" s="18"/>
+    </row>
+    <row r="111" spans="2:12">
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
       <c r="D111" s="12"/>
-      <c r="F111" s="18"/>
-      <c r="G111" s="17"/>
+      <c r="G111" s="18"/>
       <c r="H111" s="17"/>
-      <c r="K111" s="18"/>
-    </row>
-    <row r="112" spans="2:11">
+      <c r="I111" s="17"/>
+      <c r="L111" s="18"/>
+    </row>
+    <row r="112" spans="2:12">
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
-      <c r="F112" s="18"/>
-      <c r="G112" s="17"/>
+      <c r="G112" s="18"/>
       <c r="H112" s="17"/>
-      <c r="K112" s="18"/>
-    </row>
-    <row r="113" spans="2:11">
+      <c r="I112" s="17"/>
+      <c r="L112" s="18"/>
+    </row>
+    <row r="113" spans="2:12">
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
       <c r="D113" s="12"/>
-      <c r="F113" s="18"/>
-      <c r="G113" s="17"/>
+      <c r="G113" s="18"/>
       <c r="H113" s="17"/>
-      <c r="K113" s="18"/>
-    </row>
-    <row r="114" spans="2:11">
+      <c r="I113" s="17"/>
+      <c r="L113" s="18"/>
+    </row>
+    <row r="114" spans="2:12">
       <c r="B114" s="12"/>
       <c r="C114" s="12"/>
       <c r="D114" s="12"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="17"/>
+      <c r="G114" s="18"/>
       <c r="H114" s="17"/>
-      <c r="K114" s="18"/>
-    </row>
-    <row r="115" spans="2:11">
+      <c r="I114" s="17"/>
+      <c r="L114" s="18"/>
+    </row>
+    <row r="115" spans="2:12">
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
       <c r="D115" s="12"/>
-      <c r="F115" s="18"/>
-      <c r="G115" s="17"/>
+      <c r="G115" s="18"/>
       <c r="H115" s="17"/>
-      <c r="K115" s="18"/>
-    </row>
-    <row r="116" spans="2:11">
+      <c r="I115" s="17"/>
+      <c r="L115" s="18"/>
+    </row>
+    <row r="116" spans="2:12">
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
       <c r="D116" s="12"/>
-      <c r="F116" s="18"/>
-      <c r="G116" s="17"/>
+      <c r="G116" s="18"/>
       <c r="H116" s="17"/>
-      <c r="K116" s="18"/>
-    </row>
-    <row r="117" spans="2:11">
+      <c r="I116" s="17"/>
+      <c r="L116" s="18"/>
+    </row>
+    <row r="117" spans="2:12">
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
       <c r="D117" s="12"/>
-      <c r="F117" s="18"/>
-      <c r="G117" s="17"/>
+      <c r="G117" s="18"/>
       <c r="H117" s="17"/>
-      <c r="K117" s="18"/>
-    </row>
-    <row r="118" spans="2:11">
+      <c r="I117" s="17"/>
+      <c r="L117" s="18"/>
+    </row>
+    <row r="118" spans="2:12">
       <c r="B118" s="12"/>
       <c r="C118" s="12"/>
       <c r="D118" s="12"/>
-      <c r="F118" s="18"/>
-      <c r="G118" s="17"/>
+      <c r="G118" s="18"/>
       <c r="H118" s="17"/>
-      <c r="K118" s="18"/>
-    </row>
-    <row r="119" spans="2:11">
+      <c r="I118" s="17"/>
+      <c r="L118" s="18"/>
+    </row>
+    <row r="119" spans="2:12">
       <c r="B119" s="12"/>
       <c r="C119" s="12"/>
       <c r="D119" s="12"/>
-      <c r="F119" s="18"/>
-      <c r="G119" s="17"/>
+      <c r="G119" s="18"/>
       <c r="H119" s="17"/>
-      <c r="K119" s="18"/>
-    </row>
-    <row r="120" spans="2:11">
+      <c r="I119" s="17"/>
+      <c r="L119" s="18"/>
+    </row>
+    <row r="120" spans="2:12">
       <c r="B120" s="12"/>
       <c r="C120" s="12"/>
       <c r="D120" s="12"/>
-      <c r="F120" s="18"/>
-      <c r="G120" s="17"/>
+      <c r="G120" s="18"/>
       <c r="H120" s="17"/>
-      <c r="K120" s="18"/>
-    </row>
-    <row r="121" spans="2:11">
+      <c r="I120" s="17"/>
+      <c r="L120" s="18"/>
+    </row>
+    <row r="121" spans="2:12">
       <c r="B121" s="12"/>
       <c r="C121" s="12"/>
       <c r="D121" s="12"/>
-      <c r="F121" s="18"/>
-      <c r="G121" s="17"/>
+      <c r="G121" s="18"/>
       <c r="H121" s="17"/>
-      <c r="K121" s="18"/>
-    </row>
-    <row r="122" spans="2:11">
+      <c r="I121" s="17"/>
+      <c r="L121" s="18"/>
+    </row>
+    <row r="122" spans="2:12">
       <c r="B122" s="12"/>
       <c r="C122" s="12"/>
       <c r="D122" s="12"/>
-      <c r="F122" s="18"/>
-      <c r="G122" s="17"/>
+      <c r="G122" s="18"/>
       <c r="H122" s="17"/>
-      <c r="K122" s="18"/>
-    </row>
-    <row r="123" spans="2:11">
+      <c r="I122" s="17"/>
+      <c r="L122" s="18"/>
+    </row>
+    <row r="123" spans="2:12">
       <c r="B123" s="12"/>
       <c r="C123" s="12"/>
       <c r="D123" s="12"/>
-      <c r="F123" s="18"/>
-      <c r="G123" s="17"/>
+      <c r="G123" s="18"/>
       <c r="H123" s="17"/>
-      <c r="K123" s="18"/>
-    </row>
-    <row r="124" spans="2:11">
+      <c r="I123" s="17"/>
+      <c r="L123" s="18"/>
+    </row>
+    <row r="124" spans="2:12">
       <c r="B124" s="12"/>
       <c r="C124" s="12"/>
       <c r="D124" s="12"/>
-      <c r="F124" s="18"/>
-      <c r="G124" s="17"/>
+      <c r="G124" s="18"/>
       <c r="H124" s="17"/>
-      <c r="K124" s="18"/>
-    </row>
-    <row r="125" spans="2:11">
+      <c r="I124" s="17"/>
+      <c r="L124" s="18"/>
+    </row>
+    <row r="125" spans="2:12">
       <c r="B125" s="12"/>
       <c r="C125" s="12"/>
       <c r="D125" s="12"/>
-      <c r="F125" s="18"/>
-      <c r="G125" s="17"/>
+      <c r="G125" s="18"/>
       <c r="H125" s="17"/>
-      <c r="K125" s="18"/>
-    </row>
-    <row r="126" spans="2:11">
+      <c r="I125" s="17"/>
+      <c r="L125" s="18"/>
+    </row>
+    <row r="126" spans="2:12">
       <c r="B126" s="12"/>
       <c r="C126" s="12"/>
       <c r="D126" s="12"/>
-      <c r="F126" s="18"/>
-      <c r="G126" s="17"/>
+      <c r="G126" s="18"/>
       <c r="H126" s="17"/>
-      <c r="K126" s="18"/>
-    </row>
-    <row r="127" spans="2:11">
+      <c r="I126" s="17"/>
+      <c r="L126" s="18"/>
+    </row>
+    <row r="127" spans="2:12">
       <c r="B127" s="12"/>
       <c r="C127" s="12"/>
       <c r="D127" s="12"/>
-      <c r="F127" s="18"/>
-      <c r="G127" s="17"/>
+      <c r="G127" s="18"/>
       <c r="H127" s="17"/>
-      <c r="K127" s="18"/>
-    </row>
-    <row r="128" spans="2:11">
+      <c r="I127" s="17"/>
+      <c r="L127" s="18"/>
+    </row>
+    <row r="128" spans="2:12">
       <c r="B128" s="12"/>
       <c r="C128" s="12"/>
       <c r="D128" s="12"/>
-      <c r="F128" s="18"/>
-      <c r="G128" s="17"/>
+      <c r="G128" s="18"/>
       <c r="H128" s="17"/>
-      <c r="K128" s="18"/>
-    </row>
-    <row r="129" spans="2:11">
+      <c r="I128" s="17"/>
+      <c r="L128" s="18"/>
+    </row>
+    <row r="129" spans="2:12">
       <c r="B129" s="12"/>
       <c r="C129" s="12"/>
       <c r="D129" s="12"/>
-      <c r="F129" s="18"/>
-      <c r="G129" s="17"/>
+      <c r="G129" s="18"/>
       <c r="H129" s="17"/>
-      <c r="K129" s="18"/>
-    </row>
-    <row r="130" spans="2:11">
+      <c r="I129" s="17"/>
+      <c r="L129" s="18"/>
+    </row>
+    <row r="130" spans="2:12">
       <c r="B130" s="12"/>
       <c r="C130" s="12"/>
       <c r="D130" s="12"/>
-      <c r="F130" s="18"/>
-      <c r="G130" s="17"/>
+      <c r="G130" s="18"/>
       <c r="H130" s="17"/>
-      <c r="K130" s="18"/>
-    </row>
-    <row r="131" spans="2:11">
+      <c r="I130" s="17"/>
+      <c r="L130" s="18"/>
+    </row>
+    <row r="131" spans="2:12">
       <c r="B131" s="12"/>
       <c r="C131" s="12"/>
       <c r="D131" s="12"/>
-      <c r="F131" s="18"/>
-      <c r="G131" s="17"/>
+      <c r="G131" s="18"/>
       <c r="H131" s="17"/>
-      <c r="K131" s="18"/>
-    </row>
-    <row r="132" spans="2:11">
+      <c r="I131" s="17"/>
+      <c r="L131" s="18"/>
+    </row>
+    <row r="132" spans="2:12">
       <c r="B132" s="12"/>
       <c r="C132" s="12"/>
       <c r="D132" s="12"/>
-      <c r="F132" s="18"/>
-      <c r="G132" s="17"/>
+      <c r="G132" s="18"/>
       <c r="H132" s="17"/>
-      <c r="K132" s="18"/>
-    </row>
-    <row r="133" spans="2:11">
+      <c r="I132" s="17"/>
+      <c r="L132" s="18"/>
+    </row>
+    <row r="133" spans="2:12">
       <c r="B133" s="12"/>
       <c r="C133" s="12"/>
       <c r="D133" s="12"/>
-      <c r="F133" s="18"/>
-      <c r="G133" s="17"/>
+      <c r="G133" s="18"/>
       <c r="H133" s="17"/>
-      <c r="K133" s="18"/>
-    </row>
-    <row r="134" spans="2:11">
+      <c r="I133" s="17"/>
+      <c r="L133" s="18"/>
+    </row>
+    <row r="134" spans="2:12">
       <c r="B134" s="12"/>
       <c r="C134" s="12"/>
       <c r="D134" s="12"/>
-      <c r="F134" s="18"/>
-      <c r="G134" s="20"/>
+      <c r="G134" s="18"/>
       <c r="H134" s="20"/>
-      <c r="K134" s="18"/>
-    </row>
-    <row r="135" spans="2:11">
+      <c r="I134" s="20"/>
+      <c r="L134" s="18"/>
+    </row>
+    <row r="135" spans="2:12">
       <c r="B135" s="12"/>
       <c r="C135" s="12"/>
       <c r="D135" s="12"/>
       <c r="E135" s="16"/>
-      <c r="F135" s="18"/>
-      <c r="G135" s="17"/>
+      <c r="F135" s="16"/>
+      <c r="G135" s="18"/>
       <c r="H135" s="17"/>
-      <c r="K135" s="18"/>
-    </row>
-    <row r="136" spans="2:11">
+      <c r="I135" s="17"/>
+      <c r="L135" s="18"/>
+    </row>
+    <row r="136" spans="2:12">
       <c r="B136" s="12"/>
       <c r="C136" s="12"/>
       <c r="D136" s="12"/>
-      <c r="F136" s="18"/>
-      <c r="G136" s="17"/>
+      <c r="G136" s="18"/>
       <c r="H136" s="17"/>
-      <c r="K136" s="18"/>
-    </row>
-    <row r="137" spans="2:11">
+      <c r="I136" s="17"/>
+      <c r="L136" s="18"/>
+    </row>
+    <row r="137" spans="2:12">
       <c r="B137" s="12"/>
       <c r="C137" s="12"/>
       <c r="D137" s="12"/>
-      <c r="F137" s="18"/>
-      <c r="G137" s="17"/>
+      <c r="G137" s="18"/>
       <c r="H137" s="17"/>
-      <c r="K137" s="18"/>
-    </row>
-    <row r="138" spans="2:11">
+      <c r="I137" s="17"/>
+      <c r="L137" s="18"/>
+    </row>
+    <row r="138" spans="2:12">
       <c r="B138" s="12"/>
       <c r="C138" s="12"/>
       <c r="D138" s="12"/>
-      <c r="F138" s="18"/>
-      <c r="G138" s="17"/>
+      <c r="G138" s="18"/>
       <c r="H138" s="17"/>
-      <c r="K138" s="18"/>
-    </row>
-    <row r="139" spans="2:11">
+      <c r="I138" s="17"/>
+      <c r="L138" s="18"/>
+    </row>
+    <row r="139" spans="2:12">
       <c r="B139" s="12"/>
       <c r="C139" s="12"/>
       <c r="D139" s="12"/>
-      <c r="F139" s="18"/>
-      <c r="G139" s="17"/>
+      <c r="G139" s="18"/>
       <c r="H139" s="17"/>
-      <c r="K139" s="18"/>
-    </row>
-    <row r="140" spans="2:11">
+      <c r="I139" s="17"/>
+      <c r="L139" s="18"/>
+    </row>
+    <row r="140" spans="2:12">
       <c r="B140" s="12"/>
       <c r="C140" s="12"/>
       <c r="D140" s="12"/>
-      <c r="F140" s="18"/>
-      <c r="G140" s="17"/>
+      <c r="G140" s="18"/>
       <c r="H140" s="17"/>
-      <c r="K140" s="18"/>
-    </row>
-    <row r="141" spans="2:11">
+      <c r="I140" s="17"/>
+      <c r="L140" s="18"/>
+    </row>
+    <row r="141" spans="2:12">
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
       <c r="D141" s="12"/>
-      <c r="F141" s="18"/>
-      <c r="G141" s="17"/>
+      <c r="G141" s="18"/>
       <c r="H141" s="17"/>
-      <c r="K141" s="18"/>
-    </row>
-    <row r="142" spans="2:11">
+      <c r="I141" s="17"/>
+      <c r="L141" s="18"/>
+    </row>
+    <row r="142" spans="2:12">
       <c r="B142" s="12"/>
       <c r="C142" s="12"/>
       <c r="D142" s="12"/>
-      <c r="F142" s="18"/>
-      <c r="G142" s="17"/>
+      <c r="G142" s="18"/>
       <c r="H142" s="17"/>
-      <c r="K142" s="18"/>
-    </row>
-    <row r="143" spans="2:11">
+      <c r="I142" s="17"/>
+      <c r="L142" s="18"/>
+    </row>
+    <row r="143" spans="2:12">
       <c r="B143" s="12"/>
       <c r="C143" s="12"/>
       <c r="D143" s="12"/>
-      <c r="F143" s="18"/>
-      <c r="G143" s="17"/>
+      <c r="G143" s="18"/>
       <c r="H143" s="17"/>
-      <c r="K143" s="18"/>
-    </row>
-    <row r="144" spans="2:11">
+      <c r="I143" s="17"/>
+      <c r="L143" s="18"/>
+    </row>
+    <row r="144" spans="2:12">
       <c r="B144" s="12"/>
       <c r="C144" s="12"/>
       <c r="D144" s="12"/>
-      <c r="F144" s="18"/>
-      <c r="G144" s="17"/>
+      <c r="G144" s="18"/>
       <c r="H144" s="17"/>
-      <c r="K144" s="18"/>
-    </row>
-    <row r="145" spans="2:11">
+      <c r="I144" s="17"/>
+      <c r="L144" s="18"/>
+    </row>
+    <row r="145" spans="2:12">
       <c r="B145" s="12"/>
       <c r="C145" s="12"/>
       <c r="D145" s="12"/>
-      <c r="F145" s="18"/>
-      <c r="G145" s="17"/>
+      <c r="G145" s="18"/>
       <c r="H145" s="17"/>
-      <c r="K145" s="18"/>
-    </row>
-    <row r="146" spans="2:11">
+      <c r="I145" s="17"/>
+      <c r="L145" s="18"/>
+    </row>
+    <row r="146" spans="2:12">
       <c r="B146" s="12"/>
       <c r="C146" s="12"/>
       <c r="D146" s="12"/>
-      <c r="F146" s="18"/>
-      <c r="G146" s="17"/>
+      <c r="G146" s="18"/>
       <c r="H146" s="17"/>
-      <c r="K146" s="18"/>
-    </row>
-    <row r="147" spans="2:11">
+      <c r="I146" s="17"/>
+      <c r="L146" s="18"/>
+    </row>
+    <row r="147" spans="2:12">
       <c r="B147" s="12"/>
       <c r="C147" s="12"/>
       <c r="D147" s="12"/>
-      <c r="F147" s="18"/>
-      <c r="G147" s="17"/>
+      <c r="G147" s="18"/>
       <c r="H147" s="17"/>
-      <c r="K147" s="18"/>
-    </row>
-    <row r="148" spans="2:11">
+      <c r="I147" s="17"/>
+      <c r="L147" s="18"/>
+    </row>
+    <row r="148" spans="2:12">
       <c r="B148" s="12"/>
       <c r="C148" s="12"/>
       <c r="D148" s="12"/>
-      <c r="F148" s="18"/>
-      <c r="G148" s="17"/>
+      <c r="G148" s="18"/>
       <c r="H148" s="17"/>
-      <c r="K148" s="18"/>
-    </row>
-    <row r="149" spans="2:11">
+      <c r="I148" s="17"/>
+      <c r="L148" s="18"/>
+    </row>
+    <row r="149" spans="2:12">
       <c r="B149" s="12"/>
       <c r="C149" s="12"/>
       <c r="D149" s="12"/>
-      <c r="F149" s="18"/>
-      <c r="G149" s="17"/>
+      <c r="G149" s="18"/>
       <c r="H149" s="17"/>
-      <c r="K149" s="18"/>
-    </row>
-    <row r="150" spans="2:11">
+      <c r="I149" s="17"/>
+      <c r="L149" s="18"/>
+    </row>
+    <row r="150" spans="2:12">
       <c r="B150" s="12"/>
       <c r="C150" s="12"/>
       <c r="D150" s="12"/>
-      <c r="F150" s="18"/>
-      <c r="G150" s="17"/>
+      <c r="G150" s="18"/>
       <c r="H150" s="17"/>
-      <c r="K150" s="18"/>
-    </row>
-    <row r="151" spans="2:11">
+      <c r="I150" s="17"/>
+      <c r="L150" s="18"/>
+    </row>
+    <row r="151" spans="2:12">
       <c r="B151" s="12"/>
       <c r="C151" s="12"/>
       <c r="D151" s="12"/>
-      <c r="F151" s="18"/>
-      <c r="G151" s="17"/>
+      <c r="G151" s="18"/>
       <c r="H151" s="17"/>
-      <c r="K151" s="18"/>
-    </row>
-    <row r="152" spans="2:11">
+      <c r="I151" s="17"/>
+      <c r="L151" s="18"/>
+    </row>
+    <row r="152" spans="2:12">
       <c r="B152" s="12"/>
       <c r="C152" s="12"/>
       <c r="D152" s="12"/>
-      <c r="F152" s="18"/>
-      <c r="G152" s="17"/>
+      <c r="G152" s="18"/>
       <c r="H152" s="17"/>
-      <c r="K152" s="18"/>
-    </row>
-    <row r="153" spans="2:11">
+      <c r="I152" s="17"/>
+      <c r="L152" s="18"/>
+    </row>
+    <row r="153" spans="2:12">
       <c r="B153" s="12"/>
       <c r="C153" s="12"/>
       <c r="D153" s="12"/>
-      <c r="F153" s="18"/>
-      <c r="G153" s="17"/>
+      <c r="G153" s="18"/>
       <c r="H153" s="17"/>
-      <c r="K153" s="18"/>
-    </row>
-    <row r="154" spans="2:11">
+      <c r="I153" s="17"/>
+      <c r="L153" s="18"/>
+    </row>
+    <row r="154" spans="2:12">
       <c r="B154" s="12"/>
       <c r="C154" s="12"/>
       <c r="D154" s="12"/>
-      <c r="F154" s="18"/>
-      <c r="G154" s="17"/>
+      <c r="G154" s="18"/>
       <c r="H154" s="17"/>
-      <c r="K154" s="18"/>
-    </row>
-    <row r="155" spans="2:11">
+      <c r="I154" s="17"/>
+      <c r="L154" s="18"/>
+    </row>
+    <row r="155" spans="2:12">
       <c r="B155" s="12"/>
       <c r="C155" s="12"/>
       <c r="D155" s="12"/>
-      <c r="F155" s="18"/>
-      <c r="G155" s="17"/>
+      <c r="G155" s="18"/>
       <c r="H155" s="17"/>
-      <c r="K155" s="18"/>
-    </row>
-    <row r="156" spans="2:11">
+      <c r="I155" s="17"/>
+      <c r="L155" s="18"/>
+    </row>
+    <row r="156" spans="2:12">
       <c r="B156" s="12"/>
       <c r="C156" s="12"/>
       <c r="D156" s="12"/>
-      <c r="F156" s="18"/>
-      <c r="G156" s="17"/>
+      <c r="G156" s="18"/>
       <c r="H156" s="17"/>
-      <c r="K156" s="18"/>
-    </row>
-    <row r="157" spans="2:11">
+      <c r="I156" s="17"/>
+      <c r="L156" s="18"/>
+    </row>
+    <row r="157" spans="2:12">
       <c r="B157" s="12"/>
       <c r="C157" s="12"/>
       <c r="D157" s="12"/>
-      <c r="F157" s="18"/>
-      <c r="G157" s="17"/>
+      <c r="G157" s="18"/>
       <c r="H157" s="17"/>
-      <c r="K157" s="18"/>
-    </row>
-    <row r="158" spans="2:11">
+      <c r="I157" s="17"/>
+      <c r="L157" s="18"/>
+    </row>
+    <row r="158" spans="2:12">
       <c r="B158" s="12"/>
       <c r="C158" s="12"/>
       <c r="D158" s="12"/>
-      <c r="F158" s="18"/>
-      <c r="G158" s="17"/>
+      <c r="G158" s="18"/>
       <c r="H158" s="17"/>
-      <c r="K158" s="18"/>
-    </row>
-    <row r="159" spans="2:11">
+      <c r="I158" s="17"/>
+      <c r="L158" s="18"/>
+    </row>
+    <row r="159" spans="2:12">
       <c r="B159" s="12"/>
       <c r="C159" s="12"/>
       <c r="D159" s="12"/>
-      <c r="F159" s="18"/>
-      <c r="G159" s="17"/>
+      <c r="G159" s="18"/>
       <c r="H159" s="17"/>
-      <c r="K159" s="18"/>
-    </row>
-    <row r="160" spans="2:11">
+      <c r="I159" s="17"/>
+      <c r="L159" s="18"/>
+    </row>
+    <row r="160" spans="2:12">
       <c r="B160" s="12"/>
       <c r="C160" s="12"/>
       <c r="D160" s="12"/>
-      <c r="F160" s="18"/>
-      <c r="G160" s="17"/>
+      <c r="G160" s="18"/>
       <c r="H160" s="17"/>
-      <c r="K160" s="18"/>
-    </row>
-    <row r="161" spans="2:11">
+      <c r="I160" s="17"/>
+      <c r="L160" s="18"/>
+    </row>
+    <row r="161" spans="2:12">
       <c r="B161" s="12"/>
       <c r="C161" s="12"/>
       <c r="D161" s="12"/>
-      <c r="F161" s="18"/>
-      <c r="G161" s="17"/>
+      <c r="G161" s="18"/>
       <c r="H161" s="17"/>
-      <c r="K161" s="18"/>
-    </row>
-    <row r="162" spans="2:11">
+      <c r="I161" s="17"/>
+      <c r="L161" s="18"/>
+    </row>
+    <row r="162" spans="2:12">
       <c r="B162" s="12"/>
       <c r="C162" s="12"/>
       <c r="D162" s="12"/>
-      <c r="F162" s="18"/>
-      <c r="G162" s="17"/>
+      <c r="G162" s="18"/>
       <c r="H162" s="17"/>
-      <c r="K162" s="18"/>
-    </row>
-    <row r="163" spans="2:11">
+      <c r="I162" s="17"/>
+      <c r="L162" s="18"/>
+    </row>
+    <row r="163" spans="2:12">
       <c r="B163" s="12"/>
       <c r="C163" s="12"/>
       <c r="D163" s="12"/>
-      <c r="F163" s="18"/>
-      <c r="G163" s="17"/>
+      <c r="G163" s="18"/>
       <c r="H163" s="17"/>
-      <c r="K163" s="18"/>
-    </row>
-    <row r="164" spans="2:11">
+      <c r="I163" s="17"/>
+      <c r="L163" s="18"/>
+    </row>
+    <row r="164" spans="2:12">
       <c r="B164" s="12"/>
       <c r="C164" s="12"/>
       <c r="D164" s="12"/>
-      <c r="F164" s="18"/>
-      <c r="G164" s="17"/>
+      <c r="G164" s="18"/>
       <c r="H164" s="17"/>
-      <c r="K164" s="18"/>
-    </row>
-    <row r="165" spans="2:11">
+      <c r="I164" s="17"/>
+      <c r="L164" s="18"/>
+    </row>
+    <row r="165" spans="2:12">
       <c r="B165" s="12"/>
       <c r="C165" s="12"/>
       <c r="D165" s="12"/>
-      <c r="F165" s="18"/>
-      <c r="G165" s="17"/>
+      <c r="G165" s="18"/>
       <c r="H165" s="17"/>
-      <c r="K165" s="18"/>
-    </row>
-    <row r="166" spans="2:11">
+      <c r="I165" s="17"/>
+      <c r="L165" s="18"/>
+    </row>
+    <row r="166" spans="2:12">
       <c r="B166" s="12"/>
       <c r="C166" s="12"/>
       <c r="D166" s="12"/>
-      <c r="F166" s="18"/>
-      <c r="G166" s="17"/>
+      <c r="G166" s="18"/>
       <c r="H166" s="17"/>
-      <c r="K166" s="18"/>
-    </row>
-    <row r="167" spans="2:11">
+      <c r="I166" s="17"/>
+      <c r="L166" s="18"/>
+    </row>
+    <row r="167" spans="2:12">
       <c r="B167" s="12"/>
       <c r="C167" s="12"/>
       <c r="D167" s="12"/>
-      <c r="F167" s="18"/>
-      <c r="G167" s="17"/>
+      <c r="G167" s="18"/>
       <c r="H167" s="17"/>
-      <c r="K167" s="18"/>
-    </row>
-    <row r="168" spans="2:11">
+      <c r="I167" s="17"/>
+      <c r="L167" s="18"/>
+    </row>
+    <row r="168" spans="2:12">
       <c r="B168" s="12"/>
       <c r="C168" s="12"/>
       <c r="D168" s="12"/>
-      <c r="F168" s="18"/>
-      <c r="G168" s="17"/>
+      <c r="G168" s="18"/>
       <c r="H168" s="17"/>
-      <c r="K168" s="18"/>
-    </row>
-    <row r="169" spans="2:11">
+      <c r="I168" s="17"/>
+      <c r="L168" s="18"/>
+    </row>
+    <row r="169" spans="2:12">
       <c r="B169" s="12"/>
       <c r="C169" s="12"/>
       <c r="D169" s="12"/>
-      <c r="F169" s="18"/>
-      <c r="G169" s="17"/>
+      <c r="G169" s="18"/>
       <c r="H169" s="17"/>
-      <c r="K169" s="18"/>
-    </row>
-    <row r="170" spans="2:11">
+      <c r="I169" s="17"/>
+      <c r="L169" s="18"/>
+    </row>
+    <row r="170" spans="2:12">
       <c r="B170" s="12"/>
       <c r="C170" s="12"/>
       <c r="D170" s="12"/>
-      <c r="F170" s="18"/>
-      <c r="G170" s="17"/>
+      <c r="G170" s="18"/>
       <c r="H170" s="17"/>
-      <c r="K170" s="18"/>
-    </row>
-    <row r="171" spans="2:11">
+      <c r="I170" s="17"/>
+      <c r="L170" s="18"/>
+    </row>
+    <row r="171" spans="2:12">
       <c r="B171" s="12"/>
       <c r="C171" s="12"/>
       <c r="D171" s="12"/>
-      <c r="F171" s="18"/>
-      <c r="G171" s="17"/>
+      <c r="G171" s="18"/>
       <c r="H171" s="17"/>
-      <c r="K171" s="18"/>
-    </row>
-    <row r="172" spans="2:11">
+      <c r="I171" s="17"/>
+      <c r="L171" s="18"/>
+    </row>
+    <row r="172" spans="2:12">
       <c r="B172" s="12"/>
       <c r="C172" s="12"/>
       <c r="D172" s="12"/>
-      <c r="F172" s="18"/>
-      <c r="G172" s="17"/>
+      <c r="G172" s="18"/>
       <c r="H172" s="17"/>
-      <c r="K172" s="18"/>
-    </row>
-    <row r="173" spans="2:11">
+      <c r="I172" s="17"/>
+      <c r="L172" s="18"/>
+    </row>
+    <row r="173" spans="2:12">
       <c r="B173" s="12"/>
       <c r="C173" s="12"/>
       <c r="D173" s="12"/>
-      <c r="F173" s="18"/>
-      <c r="G173" s="17"/>
+      <c r="G173" s="18"/>
       <c r="H173" s="17"/>
-      <c r="K173" s="18"/>
-    </row>
-    <row r="174" spans="2:11">
+      <c r="I173" s="17"/>
+      <c r="L173" s="18"/>
+    </row>
+    <row r="174" spans="2:12">
       <c r="B174" s="12"/>
       <c r="C174" s="12"/>
       <c r="D174" s="12"/>
-      <c r="F174" s="18"/>
-      <c r="G174" s="17"/>
+      <c r="G174" s="18"/>
       <c r="H174" s="17"/>
-      <c r="K174" s="18"/>
-    </row>
-    <row r="175" spans="2:11">
+      <c r="I174" s="17"/>
+      <c r="L174" s="18"/>
+    </row>
+    <row r="175" spans="2:12">
       <c r="B175" s="12"/>
       <c r="C175" s="12"/>
       <c r="D175" s="12"/>
-      <c r="F175" s="18"/>
-      <c r="G175" s="17"/>
+      <c r="G175" s="18"/>
       <c r="H175" s="17"/>
-      <c r="K175" s="18"/>
-    </row>
-    <row r="176" spans="2:11">
+      <c r="I175" s="17"/>
+      <c r="L175" s="18"/>
+    </row>
+    <row r="176" spans="2:12">
       <c r="B176" s="12"/>
       <c r="C176" s="12"/>
       <c r="D176" s="12"/>
-      <c r="F176" s="18"/>
-      <c r="G176" s="17"/>
+      <c r="G176" s="18"/>
       <c r="H176" s="17"/>
-      <c r="K176" s="18"/>
-    </row>
-    <row r="177" spans="2:11">
+      <c r="I176" s="17"/>
+      <c r="L176" s="18"/>
+    </row>
+    <row r="177" spans="2:12">
       <c r="B177" s="12"/>
       <c r="C177" s="12"/>
       <c r="D177" s="12"/>
-      <c r="F177" s="18"/>
-      <c r="G177" s="17"/>
+      <c r="G177" s="18"/>
       <c r="H177" s="17"/>
-      <c r="K177" s="18"/>
-    </row>
-    <row r="178" spans="2:11">
+      <c r="I177" s="17"/>
+      <c r="L177" s="18"/>
+    </row>
+    <row r="178" spans="2:12">
       <c r="B178" s="12"/>
       <c r="C178" s="12"/>
       <c r="D178" s="12"/>
-      <c r="F178" s="18"/>
-      <c r="G178" s="17"/>
+      <c r="G178" s="18"/>
       <c r="H178" s="17"/>
-      <c r="K178" s="18"/>
-    </row>
-    <row r="179" spans="2:11">
+      <c r="I178" s="17"/>
+      <c r="L178" s="18"/>
+    </row>
+    <row r="179" spans="2:12">
       <c r="B179" s="12"/>
       <c r="C179" s="12"/>
       <c r="D179" s="12"/>
-      <c r="F179" s="18"/>
-      <c r="G179" s="17"/>
+      <c r="G179" s="18"/>
       <c r="H179" s="17"/>
-      <c r="K179" s="18"/>
-    </row>
-    <row r="180" spans="2:11">
+      <c r="I179" s="17"/>
+      <c r="L179" s="18"/>
+    </row>
+    <row r="180" spans="2:12">
       <c r="B180" s="12"/>
       <c r="C180" s="12"/>
       <c r="D180" s="12"/>
-      <c r="F180" s="18"/>
-      <c r="G180" s="17"/>
+      <c r="G180" s="18"/>
       <c r="H180" s="17"/>
-      <c r="K180" s="18"/>
-    </row>
-    <row r="181" spans="2:11">
+      <c r="I180" s="17"/>
+      <c r="L180" s="18"/>
+    </row>
+    <row r="181" spans="2:12">
       <c r="B181" s="12"/>
       <c r="C181" s="12"/>
       <c r="D181" s="12"/>
-      <c r="F181" s="18"/>
-      <c r="G181" s="17"/>
+      <c r="G181" s="18"/>
       <c r="H181" s="17"/>
-      <c r="K181" s="18"/>
-    </row>
-    <row r="182" spans="2:11">
+      <c r="I181" s="17"/>
+      <c r="L181" s="18"/>
+    </row>
+    <row r="182" spans="2:12">
       <c r="B182" s="12"/>
       <c r="C182" s="12"/>
       <c r="D182" s="12"/>
-      <c r="F182" s="18"/>
-      <c r="G182" s="17"/>
+      <c r="G182" s="18"/>
       <c r="H182" s="17"/>
-      <c r="K182" s="18"/>
-    </row>
-    <row r="183" spans="2:11">
+      <c r="I182" s="17"/>
+      <c r="L182" s="18"/>
+    </row>
+    <row r="183" spans="2:12">
       <c r="B183" s="12"/>
       <c r="C183" s="12"/>
       <c r="D183" s="12"/>
-      <c r="F183" s="18"/>
-      <c r="G183" s="17"/>
+      <c r="G183" s="18"/>
       <c r="H183" s="17"/>
-      <c r="K183" s="18"/>
-    </row>
-    <row r="184" spans="2:11">
+      <c r="I183" s="17"/>
+      <c r="L183" s="18"/>
+    </row>
+    <row r="184" spans="2:12">
       <c r="B184" s="12"/>
       <c r="C184" s="12"/>
       <c r="D184" s="12"/>
-      <c r="F184" s="18"/>
-      <c r="G184" s="17"/>
+      <c r="G184" s="18"/>
       <c r="H184" s="17"/>
-      <c r="K184" s="18"/>
-    </row>
-    <row r="185" spans="2:11">
+      <c r="I184" s="17"/>
+      <c r="L184" s="18"/>
+    </row>
+    <row r="185" spans="2:12">
       <c r="B185" s="12"/>
       <c r="C185" s="12"/>
       <c r="D185" s="12"/>
-      <c r="F185" s="18"/>
-      <c r="K185" s="18"/>
-    </row>
-    <row r="186" spans="2:11">
+      <c r="G185" s="18"/>
+      <c r="L185" s="18"/>
+    </row>
+    <row r="186" spans="2:12">
       <c r="B186" s="12"/>
       <c r="C186" s="12"/>
       <c r="D186" s="12"/>
-      <c r="F186" s="18"/>
-      <c r="K186" s="18"/>
-    </row>
-    <row r="187" spans="2:11">
+      <c r="G186" s="18"/>
+      <c r="L186" s="18"/>
+    </row>
+    <row r="187" spans="2:12">
       <c r="B187" s="12"/>
       <c r="C187" s="12"/>
       <c r="D187" s="12"/>
-      <c r="F187" s="18"/>
-      <c r="K187" s="18"/>
-    </row>
-    <row r="188" spans="2:11">
+      <c r="G187" s="18"/>
+      <c r="L187" s="18"/>
+    </row>
+    <row r="188" spans="2:12">
       <c r="B188" s="12"/>
       <c r="C188" s="12"/>
       <c r="D188" s="12"/>
-      <c r="F188" s="18"/>
-      <c r="K188" s="18"/>
-    </row>
-    <row r="189" spans="2:11">
+      <c r="G188" s="18"/>
+      <c r="L188" s="18"/>
+    </row>
+    <row r="189" spans="2:12">
       <c r="B189" s="12"/>
       <c r="C189" s="12"/>
       <c r="D189" s="12"/>
-      <c r="F189" s="18"/>
-      <c r="K189" s="18"/>
-    </row>
-    <row r="190" spans="2:11">
+      <c r="G189" s="18"/>
+      <c r="L189" s="18"/>
+    </row>
+    <row r="190" spans="2:12">
       <c r="B190" s="12"/>
       <c r="C190" s="12"/>
       <c r="D190" s="12"/>
-      <c r="F190" s="18"/>
-      <c r="K190" s="18"/>
-    </row>
-    <row r="191" spans="2:11">
+      <c r="G190" s="18"/>
+      <c r="L190" s="18"/>
+    </row>
+    <row r="191" spans="2:12">
       <c r="B191" s="12"/>
       <c r="C191" s="12"/>
       <c r="D191" s="12"/>
-      <c r="F191" s="18"/>
-      <c r="K191" s="18"/>
-    </row>
-    <row r="192" spans="2:11">
+      <c r="G191" s="18"/>
+      <c r="L191" s="18"/>
+    </row>
+    <row r="192" spans="2:12">
       <c r="B192" s="12"/>
       <c r="C192" s="12"/>
       <c r="D192" s="12"/>
-      <c r="F192" s="18"/>
-      <c r="K192" s="18"/>
-    </row>
-    <row r="193" spans="2:11">
+      <c r="G192" s="18"/>
+      <c r="L192" s="18"/>
+    </row>
+    <row r="193" spans="2:12">
       <c r="B193" s="12"/>
       <c r="C193" s="12"/>
       <c r="D193" s="12"/>
-      <c r="F193" s="18"/>
-      <c r="K193" s="18"/>
-    </row>
-    <row r="194" spans="2:11">
+      <c r="G193" s="18"/>
+      <c r="L193" s="18"/>
+    </row>
+    <row r="194" spans="2:12">
       <c r="B194" s="12"/>
       <c r="C194" s="12"/>
       <c r="D194" s="12"/>
-      <c r="F194" s="18"/>
-      <c r="K194" s="18"/>
-    </row>
-    <row r="195" spans="2:11">
+      <c r="G194" s="18"/>
+      <c r="L194" s="18"/>
+    </row>
+    <row r="195" spans="2:12">
       <c r="B195" s="12"/>
       <c r="C195" s="12"/>
       <c r="D195" s="12"/>
-      <c r="F195" s="18"/>
-      <c r="K195" s="18"/>
-    </row>
-    <row r="196" spans="2:11">
+      <c r="G195" s="18"/>
+      <c r="L195" s="18"/>
+    </row>
+    <row r="196" spans="2:12">
       <c r="B196" s="12"/>
       <c r="C196" s="12"/>
       <c r="D196" s="12"/>
-      <c r="F196" s="18"/>
-      <c r="K196" s="18"/>
-    </row>
-    <row r="197" spans="2:11">
+      <c r="G196" s="18"/>
+      <c r="L196" s="18"/>
+    </row>
+    <row r="197" spans="2:12">
       <c r="B197" s="12"/>
       <c r="C197" s="12"/>
       <c r="D197" s="12"/>
-      <c r="F197" s="18"/>
-      <c r="K197" s="18"/>
-    </row>
-    <row r="198" spans="2:11">
+      <c r="G197" s="18"/>
+      <c r="L197" s="18"/>
+    </row>
+    <row r="198" spans="2:12">
       <c r="B198" s="12"/>
       <c r="C198" s="12"/>
       <c r="D198" s="12"/>
-      <c r="F198" s="18"/>
-      <c r="K198" s="18"/>
-    </row>
-    <row r="199" spans="2:11">
+      <c r="G198" s="18"/>
+      <c r="L198" s="18"/>
+    </row>
+    <row r="199" spans="2:12">
       <c r="B199" s="12"/>
       <c r="C199" s="12"/>
       <c r="D199" s="12"/>
-      <c r="F199" s="18"/>
-      <c r="K199" s="18"/>
-    </row>
-    <row r="200" spans="2:11">
+      <c r="G199" s="18"/>
+      <c r="L199" s="18"/>
+    </row>
+    <row r="200" spans="2:12">
       <c r="B200" s="12"/>
       <c r="C200" s="12"/>
       <c r="D200" s="12"/>
-      <c r="F200" s="18"/>
-      <c r="K200" s="18"/>
-    </row>
-    <row r="201" spans="2:11">
+      <c r="G200" s="18"/>
+      <c r="L200" s="18"/>
+    </row>
+    <row r="201" spans="2:12">
       <c r="B201" s="12"/>
       <c r="C201" s="12"/>
       <c r="D201" s="12"/>
-      <c r="F201" s="18"/>
-      <c r="K201" s="18"/>
-    </row>
-    <row r="202" spans="2:11">
+      <c r="G201" s="18"/>
+      <c r="L201" s="18"/>
+    </row>
+    <row r="202" spans="2:12">
       <c r="B202" s="12"/>
       <c r="C202" s="12"/>
       <c r="D202" s="12"/>
-      <c r="F202" s="18"/>
-      <c r="K202" s="18"/>
-    </row>
-    <row r="203" spans="2:11">
+      <c r="G202" s="18"/>
+      <c r="L202" s="18"/>
+    </row>
+    <row r="203" spans="2:12">
       <c r="B203" s="12"/>
       <c r="C203" s="12"/>
       <c r="D203" s="12"/>
-      <c r="F203" s="18"/>
-      <c r="K203" s="18"/>
-    </row>
-    <row r="204" spans="2:11">
+      <c r="G203" s="18"/>
+      <c r="L203" s="18"/>
+    </row>
+    <row r="204" spans="2:12">
       <c r="B204" s="12"/>
       <c r="C204" s="12"/>
       <c r="D204" s="12"/>
-      <c r="F204" s="18"/>
-      <c r="K204" s="18"/>
-    </row>
-    <row r="205" spans="2:11">
+      <c r="G204" s="18"/>
+      <c r="L204" s="18"/>
+    </row>
+    <row r="205" spans="2:12">
       <c r="B205" s="12"/>
       <c r="C205" s="12"/>
       <c r="D205" s="12"/>
-      <c r="F205" s="18"/>
-      <c r="K205" s="18"/>
-    </row>
-    <row r="206" spans="2:11">
+      <c r="G205" s="18"/>
+      <c r="L205" s="18"/>
+    </row>
+    <row r="206" spans="2:12">
       <c r="B206" s="12"/>
       <c r="C206" s="12"/>
       <c r="D206" s="12"/>
-      <c r="F206" s="18"/>
-      <c r="K206" s="18"/>
-    </row>
-    <row r="207" spans="2:11">
+      <c r="G206" s="18"/>
+      <c r="L206" s="18"/>
+    </row>
+    <row r="207" spans="2:12">
       <c r="B207" s="12"/>
       <c r="C207" s="12"/>
       <c r="D207" s="12"/>
-      <c r="F207" s="18"/>
-      <c r="K207" s="18"/>
-    </row>
-    <row r="208" spans="2:11">
+      <c r="G207" s="18"/>
+      <c r="L207" s="18"/>
+    </row>
+    <row r="208" spans="2:12">
       <c r="B208" s="12"/>
       <c r="C208" s="12"/>
       <c r="D208" s="12"/>
-      <c r="F208" s="18"/>
-      <c r="K208" s="18"/>
-    </row>
-    <row r="209" spans="2:11">
+      <c r="G208" s="18"/>
+      <c r="L208" s="18"/>
+    </row>
+    <row r="209" spans="2:12">
       <c r="B209" s="12"/>
       <c r="C209" s="12"/>
       <c r="D209" s="12"/>
-      <c r="F209" s="18"/>
-      <c r="K209" s="18"/>
-    </row>
-    <row r="210" spans="2:11">
+      <c r="G209" s="18"/>
+      <c r="L209" s="18"/>
+    </row>
+    <row r="210" spans="2:12">
       <c r="B210" s="12"/>
       <c r="C210" s="12"/>
       <c r="D210" s="12"/>
-      <c r="F210" s="18"/>
-      <c r="K210" s="18"/>
-    </row>
-    <row r="211" spans="2:11">
+      <c r="G210" s="18"/>
+      <c r="L210" s="18"/>
+    </row>
+    <row r="211" spans="2:12">
       <c r="B211" s="12"/>
       <c r="C211" s="12"/>
       <c r="D211" s="12"/>
-      <c r="F211" s="18"/>
-      <c r="K211" s="18"/>
-    </row>
-    <row r="212" spans="2:11">
+      <c r="G211" s="18"/>
+      <c r="L211" s="18"/>
+    </row>
+    <row r="212" spans="2:12">
       <c r="B212" s="12"/>
       <c r="C212" s="12"/>
       <c r="D212" s="12"/>
-      <c r="F212" s="18"/>
-      <c r="K212" s="18"/>
-    </row>
-    <row r="213" spans="2:11">
+      <c r="G212" s="18"/>
+      <c r="L212" s="18"/>
+    </row>
+    <row r="213" spans="2:12">
       <c r="B213" s="12"/>
       <c r="C213" s="12"/>
       <c r="D213" s="12"/>
-      <c r="F213" s="18"/>
-      <c r="K213" s="18"/>
-    </row>
-    <row r="214" spans="2:11">
+      <c r="G213" s="18"/>
+      <c r="L213" s="18"/>
+    </row>
+    <row r="214" spans="2:12">
       <c r="B214" s="12"/>
       <c r="C214" s="12"/>
       <c r="D214" s="12"/>
-      <c r="F214" s="18"/>
-      <c r="K214" s="18"/>
-    </row>
-    <row r="215" spans="2:11">
+      <c r="G214" s="18"/>
+      <c r="L214" s="18"/>
+    </row>
+    <row r="215" spans="2:12">
       <c r="B215" s="12"/>
       <c r="C215" s="12"/>
       <c r="D215" s="12"/>
-      <c r="F215" s="18"/>
-      <c r="K215" s="18"/>
-    </row>
-    <row r="216" spans="2:11">
+      <c r="G215" s="18"/>
+      <c r="L215" s="18"/>
+    </row>
+    <row r="216" spans="2:12">
       <c r="B216" s="12"/>
       <c r="C216" s="12"/>
       <c r="D216" s="12"/>
-      <c r="F216" s="18"/>
-      <c r="K216" s="18"/>
-    </row>
-    <row r="217" spans="2:11">
+      <c r="G216" s="18"/>
+      <c r="L216" s="18"/>
+    </row>
+    <row r="217" spans="2:12">
       <c r="B217" s="12"/>
       <c r="C217" s="12"/>
       <c r="D217" s="12"/>
-      <c r="F217" s="18"/>
-      <c r="K217" s="18"/>
-    </row>
-    <row r="218" spans="2:11">
+      <c r="G217" s="18"/>
+      <c r="L217" s="18"/>
+    </row>
+    <row r="218" spans="2:12">
       <c r="B218" s="12"/>
       <c r="C218" s="12"/>
       <c r="D218" s="12"/>
-      <c r="F218" s="18"/>
-      <c r="K218" s="18"/>
-    </row>
-    <row r="219" spans="2:11">
+      <c r="G218" s="18"/>
+      <c r="L218" s="18"/>
+    </row>
+    <row r="219" spans="2:12">
       <c r="B219" s="12"/>
       <c r="C219" s="12"/>
       <c r="D219" s="12"/>
-      <c r="F219" s="18"/>
-      <c r="K219" s="18"/>
-    </row>
-    <row r="220" spans="2:11">
+      <c r="G219" s="18"/>
+      <c r="L219" s="18"/>
+    </row>
+    <row r="220" spans="2:12">
       <c r="B220" s="12"/>
       <c r="C220" s="12"/>
       <c r="D220" s="12"/>
-      <c r="F220" s="18"/>
-      <c r="K220" s="18"/>
-    </row>
-    <row r="221" spans="2:11">
+      <c r="G220" s="18"/>
+      <c r="L220" s="18"/>
+    </row>
+    <row r="221" spans="2:12">
       <c r="B221" s="12"/>
       <c r="C221" s="12"/>
       <c r="D221" s="12"/>
-      <c r="F221" s="18"/>
-      <c r="K221" s="18"/>
-    </row>
-    <row r="222" spans="2:11">
+      <c r="G221" s="18"/>
+      <c r="L221" s="18"/>
+    </row>
+    <row r="222" spans="2:12">
       <c r="B222" s="12"/>
       <c r="C222" s="12"/>
       <c r="D222" s="12"/>
-      <c r="F222" s="18"/>
-      <c r="K222" s="18"/>
-    </row>
-    <row r="223" spans="2:11">
+      <c r="G222" s="18"/>
+      <c r="L222" s="18"/>
+    </row>
+    <row r="223" spans="2:12">
       <c r="B223" s="12"/>
       <c r="C223" s="12"/>
       <c r="D223" s="12"/>
-      <c r="F223" s="18"/>
-      <c r="K223" s="18"/>
-    </row>
-    <row r="224" spans="2:11">
+      <c r="G223" s="18"/>
+      <c r="L223" s="18"/>
+    </row>
+    <row r="224" spans="2:12">
       <c r="B224" s="12"/>
       <c r="C224" s="12"/>
       <c r="D224" s="12"/>
-      <c r="F224" s="18"/>
-      <c r="K224" s="18"/>
-    </row>
-    <row r="225" spans="2:11">
+      <c r="G224" s="18"/>
+      <c r="L224" s="18"/>
+    </row>
+    <row r="225" spans="2:12">
       <c r="B225" s="12"/>
       <c r="C225" s="12"/>
       <c r="D225" s="12"/>
-      <c r="F225" s="18"/>
-      <c r="K225" s="18"/>
-    </row>
-    <row r="226" spans="2:11">
+      <c r="G225" s="18"/>
+      <c r="L225" s="18"/>
+    </row>
+    <row r="226" spans="2:12">
       <c r="B226" s="12"/>
       <c r="C226" s="12"/>
       <c r="D226" s="12"/>
-      <c r="F226" s="18"/>
-      <c r="K226" s="18"/>
-    </row>
-    <row r="227" spans="2:11">
+      <c r="G226" s="18"/>
+      <c r="L226" s="18"/>
+    </row>
+    <row r="227" spans="2:12">
       <c r="B227" s="12"/>
       <c r="C227" s="12"/>
       <c r="D227" s="12"/>
-      <c r="F227" s="18"/>
-      <c r="K227" s="18"/>
-    </row>
-    <row r="228" spans="2:11">
+      <c r="G227" s="18"/>
+      <c r="L227" s="18"/>
+    </row>
+    <row r="228" spans="2:12">
       <c r="B228" s="12"/>
       <c r="C228" s="12"/>
       <c r="D228" s="12"/>
-      <c r="F228" s="18"/>
-      <c r="K228" s="18"/>
-    </row>
-    <row r="229" spans="2:11">
+      <c r="G228" s="18"/>
+      <c r="L228" s="18"/>
+    </row>
+    <row r="229" spans="2:12">
       <c r="B229" s="12"/>
       <c r="C229" s="12"/>
       <c r="D229" s="12"/>
-      <c r="F229" s="18"/>
-      <c r="K229" s="18"/>
-    </row>
-    <row r="230" spans="2:11">
+      <c r="G229" s="18"/>
+      <c r="L229" s="18"/>
+    </row>
+    <row r="230" spans="2:12">
       <c r="B230" s="12"/>
       <c r="C230" s="12"/>
       <c r="D230" s="12"/>
-      <c r="F230" s="18"/>
-      <c r="K230" s="18"/>
-    </row>
-    <row r="231" spans="2:11">
+      <c r="G230" s="18"/>
+      <c r="L230" s="18"/>
+    </row>
+    <row r="231" spans="2:12">
       <c r="B231" s="12"/>
       <c r="C231" s="12"/>
       <c r="D231" s="12"/>
-      <c r="F231" s="18"/>
-      <c r="K231" s="18"/>
-    </row>
-    <row r="232" spans="2:11">
+      <c r="G231" s="18"/>
+      <c r="L231" s="18"/>
+    </row>
+    <row r="232" spans="2:12">
       <c r="B232" s="12"/>
       <c r="C232" s="12"/>
       <c r="D232" s="12"/>
-      <c r="F232" s="18"/>
-      <c r="K232" s="18"/>
-    </row>
-    <row r="233" spans="2:11">
+      <c r="G232" s="18"/>
+      <c r="L232" s="18"/>
+    </row>
+    <row r="233" spans="2:12">
       <c r="B233" s="12"/>
       <c r="C233" s="12"/>
       <c r="D233" s="12"/>
-      <c r="F233" s="18"/>
-      <c r="K233" s="18"/>
-    </row>
-    <row r="234" spans="2:11">
+      <c r="G233" s="18"/>
+      <c r="L233" s="18"/>
+    </row>
+    <row r="234" spans="2:12">
       <c r="B234" s="12"/>
       <c r="C234" s="12"/>
       <c r="D234" s="12"/>
-      <c r="F234" s="18"/>
-      <c r="K234" s="18"/>
-    </row>
-    <row r="235" spans="2:11">
+      <c r="G234" s="18"/>
+      <c r="L234" s="18"/>
+    </row>
+    <row r="235" spans="2:12">
       <c r="B235" s="12"/>
       <c r="C235" s="12"/>
       <c r="D235" s="12"/>
-      <c r="F235" s="18"/>
-      <c r="K235" s="18"/>
-    </row>
-    <row r="236" spans="2:11">
+      <c r="G235" s="18"/>
+      <c r="L235" s="18"/>
+    </row>
+    <row r="236" spans="2:12">
       <c r="B236" s="12"/>
       <c r="C236" s="12"/>
       <c r="D236" s="12"/>
-      <c r="F236" s="18"/>
-      <c r="K236" s="18"/>
-    </row>
-    <row r="237" spans="2:11">
+      <c r="G236" s="18"/>
+      <c r="L236" s="18"/>
+    </row>
+    <row r="237" spans="2:12">
       <c r="B237" s="12"/>
       <c r="C237" s="12"/>
       <c r="D237" s="12"/>
-      <c r="F237" s="18"/>
-      <c r="K237" s="18"/>
-    </row>
-    <row r="238" spans="2:11">
+      <c r="G237" s="18"/>
+      <c r="L237" s="18"/>
+    </row>
+    <row r="238" spans="2:12">
       <c r="B238" s="12"/>
       <c r="C238" s="12"/>
       <c r="D238" s="12"/>
-      <c r="F238" s="18"/>
-      <c r="K238" s="18"/>
-    </row>
-    <row r="239" spans="2:11">
+      <c r="G238" s="18"/>
+      <c r="L238" s="18"/>
+    </row>
+    <row r="239" spans="2:12">
       <c r="B239" s="12"/>
       <c r="C239" s="12"/>
       <c r="D239" s="12"/>
-      <c r="F239" s="18"/>
-      <c r="K239" s="18"/>
-    </row>
-    <row r="240" spans="2:11">
+      <c r="G239" s="18"/>
+      <c r="L239" s="18"/>
+    </row>
+    <row r="240" spans="2:12">
       <c r="B240" s="12"/>
       <c r="C240" s="12"/>
       <c r="D240" s="12"/>
-      <c r="F240" s="18"/>
-      <c r="K240" s="18"/>
-    </row>
-    <row r="241" spans="2:11">
+      <c r="G240" s="18"/>
+      <c r="L240" s="18"/>
+    </row>
+    <row r="241" spans="2:12">
       <c r="B241" s="12"/>
       <c r="C241" s="12"/>
       <c r="D241" s="12"/>
-      <c r="F241" s="18"/>
-      <c r="K241" s="18"/>
+      <c r="G241" s="18"/>
+      <c r="L241" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>